<commit_message>
p2p and first mile
</commit_message>
<xml_diff>
--- a/Logs/jbhunt_api_tracking.xlsx
+++ b/Logs/jbhunt_api_tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>Timestamp</t>
   </si>
@@ -61,10 +61,55 @@
     <t>2025-08-10 14:23:33</t>
   </si>
   <si>
+    <t>2025-08-11 12:42:15</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:42:29</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:42:43</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:42:58</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:43:13</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:45:29</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:45:32</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:45:45</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:45:48</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:46:14</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:53:07</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:53:19</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:53:34</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:53:36</t>
+  </si>
+  <si>
+    <t>2025-08-11 12:53:50</t>
+  </si>
+  <si>
     <t>07201</t>
   </si>
   <si>
-    <t>85043</t>
+    <t>21901</t>
   </si>
   <si>
     <t>Success</t>
@@ -92,6 +137,15 @@
   </si>
   <si>
     <t>Rate: 3493.82, Carrier: JBHZ</t>
+  </si>
+  <si>
+    <t>Rate: 693.44, Carrier: JBHZ</t>
+  </si>
+  <si>
+    <t>Rate: 428.9, Carrier: JBHZ</t>
+  </si>
+  <si>
+    <t>Rate: 714.31, Carrier: JBHZ</t>
   </si>
 </sst>
 </file>
@@ -449,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,10 +543,10 @@
         <v>45007.703685</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -509,10 +563,10 @@
         <v>11025</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -529,10 +583,10 @@
         <v>45007.703685</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -549,10 +603,10 @@
         <v>11025</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -569,10 +623,10 @@
         <v>45007.703685</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -589,10 +643,10 @@
         <v>11025</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -609,10 +663,10 @@
         <v>45007.703685</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -629,10 +683,10 @@
         <v>11025</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -649,30 +703,330 @@
         <v>11025</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11">
+        <v>7201</v>
+      </c>
+      <c r="C11">
+        <v>85043</v>
+      </c>
+      <c r="D11">
+        <v>45007.703685</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12">
+        <v>29483</v>
+      </c>
+      <c r="C12">
+        <v>30567</v>
+      </c>
+      <c r="D12">
+        <v>11025</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
-        <v>45007.703685</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B13">
+        <v>29483</v>
+      </c>
+      <c r="C13">
+        <v>30567</v>
+      </c>
+      <c r="D13">
+        <v>45007.703685</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
+      <c r="B14">
+        <v>7201</v>
+      </c>
+      <c r="C14">
+        <v>8873</v>
+      </c>
+      <c r="D14">
+        <v>11025</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>7201</v>
+      </c>
+      <c r="C15">
+        <v>8873</v>
+      </c>
+      <c r="D15">
+        <v>45007.703685</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>7201</v>
+      </c>
+      <c r="C16">
+        <v>21901</v>
+      </c>
+      <c r="D16">
+        <v>45007.703685</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>29483</v>
+      </c>
+      <c r="C17">
+        <v>30567</v>
+      </c>
+      <c r="D17">
+        <v>11025</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>29483</v>
+      </c>
+      <c r="C18">
+        <v>30567</v>
+      </c>
+      <c r="D18">
+        <v>45007.703685</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>7201</v>
+      </c>
+      <c r="C19">
+        <v>8873</v>
+      </c>
+      <c r="D19">
+        <v>11025</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>7201</v>
+      </c>
+      <c r="C20">
+        <v>8873</v>
+      </c>
+      <c r="D20">
+        <v>45007.703685</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>7201</v>
+      </c>
+      <c r="C21">
+        <v>21901</v>
+      </c>
+      <c r="D21">
+        <v>45007.703685</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
         <v>25</v>
+      </c>
+      <c r="B22">
+        <v>29483</v>
+      </c>
+      <c r="C22">
+        <v>30567</v>
+      </c>
+      <c r="D22">
+        <v>11025</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>29483</v>
+      </c>
+      <c r="C23">
+        <v>30567</v>
+      </c>
+      <c r="D23">
+        <v>45007.703685</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>7201</v>
+      </c>
+      <c r="C24">
+        <v>8873</v>
+      </c>
+      <c r="D24">
+        <v>11025</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>7201</v>
+      </c>
+      <c r="C25">
+        <v>8873</v>
+      </c>
+      <c r="D25">
+        <v>45007.703685</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>45007.703685</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>